<commit_message>
[ROOT] Implement Github Actions + Fix README.md
[FIX] Update README images

[NEW] Add schematics

[ACT] Try to use github actions

[ACT] Move to the good folder

[ACT] First test of action

[GEN] Remove generated for test

[ACT] Fix variant

[ACT] 2nd test

[ACT] 3rd test

[ACT] 3rd test (really this one)

[ACT] 4th test

[ACT] 4th test (really again....)

[ACT] 5th test

[ACT] 6th test

[ACT] 7th test

[ACT] 7th test (really)

[ACT] 8th test (maybe)

[ACT] test

[ACT] Fix run

[CI] Auto-release exports files

[ACT] Fix ERC

[ACT] Fix add -f

[CI] Auto-release exports files

[PCB] Edit PCB

[CI] Auto-release exports files
</commit_message>
<xml_diff>
--- a/Export/cost/KibotTest-kicost.xlsx
+++ b/Export/cost/KibotTest-kicost.xlsx
@@ -206,7 +206,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>Sat 04 Jun 2022 05:41:55 PM CEST</t>
+    <t>Sat Jun  4 23:26:00 2022</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -221,7 +221,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2022-06-04 17:41:56</t>
+    <t>2022-06-04 23:26:02</t>
   </si>
   <si>
     <t>KiCost® v1.1.8</t>
@@ -243,6 +243,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -291,12 +297,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -324,27 +324,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -678,148 +679,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="F2" s="1" t="s">
+      <c r="B2" s="3"/>
+      <c r="F2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <f>TotalCost/BoardQty</f>
         <v>0.0</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="6">
         <f>SUM(G7:G9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="9">
         <f>CEILING(BoardQty*1,1)</f>
         <v>1</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="10" t="str">
         <f>IF(AND(ISNUMBER(E7),ISNUMBER(F7)),E7*F7,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:7" ht="30.0" customHeight="1">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="9">
         <f>CEILING(BoardQty*1,1)</f>
         <v>1</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="10" t="str">
         <f>IF(AND(ISNUMBER(E8),ISNUMBER(F8)),E8*F8,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:7" ht="30.0" customHeight="1">
+      <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="9">
         <f>CEILING(BoardQty*1,1)</f>
         <v>1</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="10" t="str">
         <f>IF(AND(ISNUMBER(E9),ISNUMBER(F9)),E9*F9,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C11">
@@ -827,7 +828,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[CI] Auto-release exports files
</commit_message>
<xml_diff>
--- a/Export/cost/KibotTest-kicost.xlsx
+++ b/Export/cost/KibotTest-kicost.xlsx
@@ -206,7 +206,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>Sat Jun  4 23:26:00 2022</t>
+    <t>Sun Jun  5 00:02:57 2022</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -221,7 +221,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2022-06-04 23:26:02</t>
+    <t>2022-06-05 00:03:00</t>
   </si>
   <si>
     <t>KiCost® v1.1.8</t>

</xml_diff>